<commit_message>
Update city LHJ files
</commit_message>
<xml_diff>
--- a/LHJ Data/E6/Clean/E6-2020-cy.xlsx
+++ b/LHJ Data/E6/Clean/E6-2020-cy.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\Population Task Force\LHJ Data\E6\Clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03A61DDF-FD15-4112-AC14-5A48C54EFC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48623BB6-D7E0-4683-A562-18A14580C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{40498B7D-AED7-479D-9C0A-B88DC391C774}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="15435" xr2:uid="{40498B7D-AED7-479D-9C0A-B88DC391C774}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="archive2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">archive2022!$A$1:$C$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$237</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="63">
   <si>
     <t>California</t>
   </si>
@@ -226,6 +228,9 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>2021</t>
+  </si>
 </sst>
 </file>
 
@@ -320,7 +325,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -344,6 +349,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{F4663794-C4CF-4DE7-B17D-5C9D262C1F7F}"/>
@@ -665,11 +682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06019EA7-A7E8-440C-937E-715FF6003195}">
-  <dimension ref="A1:H178"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DF17EE-2BF8-40BC-AD74-DCFC418889E9}">
+  <dimension ref="A1:H237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="H174" sqref="H174"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,14 +711,14 @@
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>2020</v>
-      </c>
-      <c r="C2" s="8">
-        <v>39520071</v>
+      <c r="B2" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="14">
+        <v>39541722</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -710,14 +727,14 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <v>2021</v>
-      </c>
-      <c r="C3" s="8">
-        <v>39239553</v>
+      <c r="B3" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="14">
+        <v>39246702</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -726,14 +743,14 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
-        <v>2022</v>
-      </c>
-      <c r="C4" s="8">
-        <v>39028571</v>
+      <c r="B4" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="14">
+        <v>39146273</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -742,14 +759,14 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2020</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1676458</v>
+      <c r="A5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C5" s="14">
+        <v>39109070</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -758,6 +775,3227 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1680487</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1657465</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2022</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1649975</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2023</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1656037</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="14">
+        <v>1202</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1180</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1175</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1165</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="14">
+        <v>40440</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="14">
+        <v>40262</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="14">
+        <v>40105</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C17" s="14">
+        <v>40122</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="14">
+        <v>210349</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C19" s="14">
+        <v>206121</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C20" s="14">
+        <v>206498</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C21" s="14">
+        <v>205860</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="14">
+        <v>45262</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C23" s="14">
+        <v>45011</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C24" s="14">
+        <v>44769</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C25" s="14">
+        <v>44605</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C26" s="14">
+        <v>21867</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C27" s="14">
+        <v>21884</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C28" s="14">
+        <v>21814</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C29" s="14">
+        <v>21905</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1167327</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1159901</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1150114</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C33" s="14">
+        <v>1146536</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C34" s="14">
+        <v>27645</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C35" s="14">
+        <v>27368</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C36" s="14">
+        <v>26738</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C37" s="14">
+        <v>26382</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C38" s="14">
+        <v>191522</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C39" s="14">
+        <v>191437</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C40" s="14">
+        <v>189386</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C41" s="14">
+        <v>187285</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C42" s="14">
+        <v>1007436</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="12">
+        <v>2021</v>
+      </c>
+      <c r="C43" s="14">
+        <v>1010417</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C44" s="14">
+        <v>1011462</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C45" s="14">
+        <v>1012424</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C46" s="14">
+        <v>28854</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="12">
+        <v>2021</v>
+      </c>
+      <c r="C47" s="14">
+        <v>28709</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C48" s="14">
+        <v>28449</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C49" s="14">
+        <v>28039</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C50" s="14">
+        <v>136406</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="12">
+        <v>2021</v>
+      </c>
+      <c r="C51" s="14">
+        <v>134695</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C52" s="14">
+        <v>134657</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C53" s="14">
+        <v>134388</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C54" s="14">
+        <v>180376</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="14">
+        <v>179807</v>
+      </c>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C56" s="14">
+        <v>179914</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C57" s="14">
+        <v>179639</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C58" s="14">
+        <v>18954</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="14">
+        <v>18874</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C60" s="14">
+        <v>18847</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C61" s="14">
+        <v>18731</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C62" s="14">
+        <v>905783</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="14">
+        <v>908418</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C64" s="14">
+        <v>908708</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C65" s="14">
+        <v>903372</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C66" s="14">
+        <v>152531</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" s="14">
+        <v>151751</v>
+      </c>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C68" s="14">
+        <v>151954</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C69" s="14">
+        <v>152405</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C70" s="14">
+        <v>67864</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="14">
+        <v>67714</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C72" s="14">
+        <v>67206</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C73" s="14">
+        <v>66446</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C74" s="14">
+        <v>31926</v>
+      </c>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="14">
+        <v>31054</v>
+      </c>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C76" s="14">
+        <v>29544</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C77" s="14">
+        <v>28232</v>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C78" s="14">
+        <v>10014848</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79" s="14">
+        <v>9908772</v>
+      </c>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C80" s="14">
+        <v>9840925</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C81" s="14">
+        <v>9825708</v>
+      </c>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C82" s="14">
+        <v>156422</v>
+      </c>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" s="14">
+        <v>157008</v>
+      </c>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C84" s="14">
+        <v>157287</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C85" s="14">
+        <v>158457</v>
+      </c>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C86" s="14">
+        <v>262161</v>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C87" s="14">
+        <v>258719</v>
+      </c>
+      <c r="D87" s="4"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B88" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C88" s="14">
+        <v>255851</v>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C89" s="14">
+        <v>254744</v>
+      </c>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C90" s="14">
+        <v>17102</v>
+      </c>
+      <c r="D90" s="4"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" s="14">
+        <v>17015</v>
+      </c>
+      <c r="D91" s="4"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B92" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C92" s="14">
+        <v>16943</v>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C93" s="14">
+        <v>16860</v>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C94" s="14">
+        <v>91319</v>
+      </c>
+      <c r="D94" s="4"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C95" s="14">
+        <v>90854</v>
+      </c>
+      <c r="D95" s="4"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C96" s="14">
+        <v>89960</v>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C97" s="14">
+        <v>89316</v>
+      </c>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C98" s="14">
+        <v>281128</v>
+      </c>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" s="14">
+        <v>281695</v>
+      </c>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C100" s="14">
+        <v>285140</v>
+      </c>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B101" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C101" s="14">
+        <v>285600</v>
+      </c>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B102" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C102" s="14">
+        <v>8686</v>
+      </c>
+      <c r="D102" s="4"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C103" s="14">
+        <v>8542</v>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C104" s="14">
+        <v>8517</v>
+      </c>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C105" s="14">
+        <v>8446</v>
+      </c>
+      <c r="D105" s="4"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C106" s="14">
+        <v>13368</v>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C107" s="14">
+        <v>13276</v>
+      </c>
+      <c r="D107" s="4"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C108" s="14">
+        <v>13185</v>
+      </c>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C109" s="14">
+        <v>13273</v>
+      </c>
+      <c r="D109" s="4"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B110" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C110" s="14">
+        <v>439762</v>
+      </c>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C111" s="14">
+        <v>438349</v>
+      </c>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="10"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C112" s="14">
+        <v>436843</v>
+      </c>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C113" s="14">
+        <v>436476</v>
+      </c>
+      <c r="D113" s="4"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B114" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C114" s="14">
+        <v>138058</v>
+      </c>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="10"/>
+      <c r="G114" s="10"/>
+      <c r="H114" s="10"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C115" s="14">
+        <v>136891</v>
+      </c>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C116" s="14">
+        <v>135497</v>
+      </c>
+      <c r="D116" s="4"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="4"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="4"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B117" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C117" s="14">
+        <v>134484</v>
+      </c>
+      <c r="D117" s="4"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B118" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C118" s="14">
+        <v>102648</v>
+      </c>
+      <c r="D118" s="4"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C119" s="14">
+        <v>102435</v>
+      </c>
+      <c r="D119" s="4"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10"/>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B120" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C120" s="14">
+        <v>101137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B121" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C121" s="14">
+        <v>100400</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B122" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C122" s="14">
+        <v>3188652</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C123" s="14">
+        <v>3164848</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C124" s="14">
+        <v>3154042</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B125" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C125" s="14">
+        <v>3142277</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B126" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C126" s="14">
+        <v>406495</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C127" s="14">
+        <v>408769</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B128" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C128" s="14">
+        <v>409692</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B129" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C129" s="14">
+        <v>410706</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B130" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C130" s="14">
+        <v>19871</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C131" s="14">
+        <v>19733</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B132" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C132" s="14">
+        <v>19280</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B133" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C133" s="14">
+        <v>18955</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B134" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C134" s="14">
+        <v>2423288</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C135" s="14">
+        <v>2429268</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B136" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C136" s="14">
+        <v>2432203</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B137" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C137" s="14">
+        <v>2431254</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B138" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C138" s="14">
+        <v>1587542</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" s="14">
+        <v>1583966</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B140" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C140" s="14">
+        <v>1578644</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B141" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C141" s="14">
+        <v>1581831</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B142" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C142" s="14">
+        <v>64450</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C143" s="14">
+        <v>65182</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B144" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C144" s="14">
+        <v>65481</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B145" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C145" s="14">
+        <v>65082</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B146" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C146" s="14">
+        <v>2185348</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C147" s="14">
+        <v>2183756</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B148" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C148" s="14">
+        <v>2179263</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B149" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C149" s="14">
+        <v>2170593</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B150" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C150" s="14">
+        <v>3304801</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B151" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C151" s="14">
+        <v>3285268</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B152" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C152" s="14">
+        <v>3293911</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C153" s="14">
+        <v>3297860</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B154" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C154" s="14">
+        <v>870734</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B155" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C155" s="14">
+        <v>841721</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B156" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C156" s="14">
+        <v>843094</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B157" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C157" s="14">
+        <v>848019</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B158" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C158" s="14">
+        <v>779968</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C159" s="14">
+        <v>781946</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B160" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C160" s="14">
+        <v>784017</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B161" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C161" s="14">
+        <v>784528</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B162" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C162" s="14">
+        <v>282671</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C163" s="14">
+        <v>278527</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B164" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C164" s="14">
+        <v>280629</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B165" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C165" s="14">
+        <v>280251</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B166" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C166" s="14">
+        <v>762754</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B167" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C167" s="14">
+        <v>749908</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B168" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C168" s="14">
+        <v>746262</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B169" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C169" s="14">
+        <v>749075</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B170" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C170" s="14">
+        <v>447860</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B171" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C171" s="14">
+        <v>439100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B172" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C172" s="14">
+        <v>443956</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B173" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C173" s="14">
+        <v>442614</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B174" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C174" s="14">
+        <v>1926546</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B175" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C175" s="14">
+        <v>1899926</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B176" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C176" s="14">
+        <v>1903274</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B177" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C177" s="14">
+        <v>1911749</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B178" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C178" s="14">
+        <v>271222</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B179" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C179" s="14">
+        <v>263170</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B180" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C180" s="14">
+        <v>265158</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B181" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C181" s="14">
+        <v>263101</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B182" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C182" s="14">
+        <v>182029</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B183" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C183" s="14">
+        <v>181374</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B184" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C184" s="14">
+        <v>179786</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B185" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C185" s="14">
+        <v>178958</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B186" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C186" s="14">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B187" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C187" s="14">
+        <v>3212</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B188" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C188" s="14">
+        <v>3186</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B189" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C189" s="14">
+        <v>3152</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B190" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C190" s="14">
+        <v>43996</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B191" s="12">
+        <v>2021</v>
+      </c>
+      <c r="C191" s="14">
+        <v>43543</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B192" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C192" s="14">
+        <v>43307</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B193" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C193" s="14">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B194" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C194" s="14">
+        <v>452943</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B195" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C195" s="14">
+        <v>449539</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B196" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C196" s="14">
+        <v>447012</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B197" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C197" s="14">
+        <v>446745</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B198" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C198" s="14">
+        <v>488765</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B199" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C199" s="14">
+        <v>483300</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B200" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C200" s="14">
+        <v>481297</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B201" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C201" s="14">
+        <v>479826</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B202" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C202" s="14">
+        <v>553129</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B203" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C203" s="14">
+        <v>550885</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B204" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C204" s="14">
+        <v>547905</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B205" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C205" s="14">
+        <v>545704</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B206" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C206" s="14">
+        <v>99474</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B207" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C207" s="14">
+        <v>99020</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B208" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C208" s="14">
+        <v>98641</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B209" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C209" s="14">
+        <v>98151</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B210" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C210" s="14">
+        <v>65847</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B211" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C211" s="14">
+        <v>65424</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B212" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C212" s="14">
+        <v>64993</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B213" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C213" s="14">
+        <v>64677</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B214" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C214" s="14">
+        <v>16107</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B215" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C215" s="14">
+        <v>16009</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B216" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C216" s="14">
+        <v>15927</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B217" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C217" s="14">
+        <v>15870</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B218" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C218" s="14">
+        <v>472757</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B219" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C219" s="14">
+        <v>474780</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B220" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C220" s="14">
+        <v>474861</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B221" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C221" s="14">
+        <v>474792</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B222" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C222" s="14">
+        <v>55492</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B223" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C223" s="14">
+        <v>54690</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B224" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C224" s="14">
+        <v>53409</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B225" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C225" s="14">
+        <v>53387</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B226" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C226" s="14">
+        <v>844214</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B227" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C227" s="14">
+        <v>837619</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B228" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C228" s="14">
+        <v>830434</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B229" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C229" s="14">
+        <v>825937</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B230" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C230" s="14">
+        <v>217883</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B231" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C231" s="14">
+        <v>214339</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B232" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C232" s="14">
+        <v>221342</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B233" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C233" s="14">
+        <v>220381</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B234" s="12">
+        <v>2020</v>
+      </c>
+      <c r="C234" s="14">
+        <v>81919</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B235" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C235" s="14">
+        <v>82256</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B236" s="12">
+        <v>2022</v>
+      </c>
+      <c r="C236" s="14">
+        <v>82667</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B237" s="12">
+        <v>2023</v>
+      </c>
+      <c r="C237" s="14">
+        <v>83297</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C237" xr:uid="{E3DF17EE-2BF8-40BC-AD74-DCFC418889E9}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06019EA7-A7E8-440C-937E-715FF6003195}">
+  <dimension ref="A1:H178"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="8">
+        <v>39520071</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C3" s="8">
+        <v>39239553</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="8">
+        <v>39028571</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1676458</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated LHJ Population Data File (date updated: 2025.05.21) with newest DOF P3 Vintage 2025 (released 2025.04.25), DOF E4 2010-2020 (released May 2025), and DOF E4 2020-2025 (released May 2025)
</commit_message>
<xml_diff>
--- a/LHJ Data/E6/Clean/E6-2020-cy.xlsx
+++ b/LHJ Data/E6/Clean/E6-2020-cy.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\Population Task Force\LHJ Data\E6\Clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48623BB6-D7E0-4683-A562-18A14580C5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C4DA57-7146-46BB-800C-C5FB28F5F004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="15435" xr2:uid="{40498B7D-AED7-479D-9C0A-B88DC391C774}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{40498B7D-AED7-479D-9C0A-B88DC391C774}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="archive2022" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="archive2023" sheetId="3" r:id="rId2"/>
+    <sheet name="archive2022" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">archive2022!$A$1:$C$178</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$237</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">archive2022!$A$1:$C$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">archive2023!$A$1:$C$237</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="66">
   <si>
     <t>California</t>
   </si>
@@ -231,6 +232,15 @@
   <si>
     <t>2021</t>
   </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
 </sst>
 </file>
 
@@ -290,15 +300,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -315,6 +331,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -325,7 +415,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -361,6 +451,36 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{F4663794-C4CF-4DE7-B17D-5C9D262C1F7F}"/>
@@ -387,9 +507,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -427,7 +547,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -533,7 +653,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -675,18 +795,3293 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F57394A-25B0-4B88-9D03-C780B3D198BD}">
+  <dimension ref="A1:C297"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="17">
+        <v>39535726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="20">
+        <v>39229543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="17">
+        <v>39149809</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C5" s="20">
+        <v>39123861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="17">
+        <v>39172742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1679664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16">
+        <v>2021</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1655767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1645265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="17">
+        <v>1644199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="20">
+        <v>1644569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="20">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="17">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C15" s="20">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C16" s="17">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="20">
+        <v>40391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="17">
+        <v>40224</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C19" s="20">
+        <v>40073</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C20" s="17">
+        <v>40028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C21" s="20">
+        <v>39893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C22" s="17">
+        <v>210219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="20">
+        <v>206058</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C24" s="17">
+        <v>206183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C25" s="20">
+        <v>205741</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C26" s="17">
+        <v>206194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C27" s="20">
+        <v>45253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="17">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C29" s="20">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C30" s="17">
+        <v>44616</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C31" s="20">
+        <v>44436</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C32" s="17">
+        <v>21811</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="20">
+        <v>21899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C34" s="17">
+        <v>21902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C35" s="20">
+        <v>21981</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C36" s="17">
+        <v>22016</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C37" s="20">
+        <v>1165866</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1159660</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C39" s="20">
+        <v>1150950</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C40" s="17">
+        <v>1148745</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C41" s="20">
+        <v>1148324</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C42" s="17">
+        <v>27648</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="20">
+        <v>27352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C44" s="17">
+        <v>26513</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C45" s="20">
+        <v>26320</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C46" s="17">
+        <v>26607</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C47" s="20">
+        <v>191306</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="17">
+        <v>191671</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C49" s="20">
+        <v>190259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C50" s="17">
+        <v>189355</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C51" s="20">
+        <v>189079</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C52" s="17">
+        <v>1007099</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="20">
+        <v>1010004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C54" s="17">
+        <v>1013642</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C55" s="20">
+        <v>1017152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C56" s="17">
+        <v>1019566</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C57" s="20">
+        <v>28848</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="17">
+        <v>28687</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C59" s="20">
+        <v>28647</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C60" s="17">
+        <v>28596</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C61" s="20">
+        <v>28711</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C62" s="17">
+        <v>136193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="20">
+        <v>134709</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C64" s="17">
+        <v>134560</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C65" s="20">
+        <v>133968</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C66" s="17">
+        <v>133359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C67" s="20">
+        <v>180304</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="17">
+        <v>179707</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C69" s="20">
+        <v>180669</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C70" s="17">
+        <v>182090</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C71" s="20">
+        <v>183812</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C72" s="17">
+        <v>18955</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C73" s="20">
+        <v>18881</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C74" s="17">
+        <v>18856</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C75" s="20">
+        <v>18740</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C76" s="17">
+        <v>18644</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B77" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C77" s="20">
+        <v>905446</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="17">
+        <v>908274</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C79" s="20">
+        <v>910910</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C80" s="17">
+        <v>908297</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C81" s="20">
+        <v>911180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C82" s="17">
+        <v>152408</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C83" s="20">
+        <v>151674</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C84" s="17">
+        <v>151865</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C85" s="20">
+        <v>152548</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C86" s="17">
+        <v>152833</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B87" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C87" s="20">
+        <v>67833</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="17">
+        <v>67630</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C89" s="20">
+        <v>67363</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C90" s="17">
+        <v>66875</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C91" s="20">
+        <v>66918</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C92" s="17">
+        <v>31917</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="20">
+        <v>31049</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C94" s="17">
+        <v>29711</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B95" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C95" s="20">
+        <v>28137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B96" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C96" s="17">
+        <v>28027</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B97" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C97" s="20">
+        <v>10019274</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" s="17">
+        <v>9909370</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B99" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C99" s="20">
+        <v>9839078</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B100" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C100" s="17">
+        <v>9811463</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B101" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C101" s="20">
+        <v>9822800</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C102" s="17">
+        <v>156290</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C103" s="20">
+        <v>156963</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C104" s="17">
+        <v>157735</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C105" s="20">
+        <v>159892</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C106" s="17">
+        <v>160788</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C107" s="20">
+        <v>261805</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C108" s="17">
+        <v>258668</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C109" s="20">
+        <v>255847</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C110" s="17">
+        <v>254301</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C111" s="20">
+        <v>252899</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B112" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C112" s="17">
+        <v>17098</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B113" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C113" s="20">
+        <v>17016</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B114" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C114" s="17">
+        <v>16942</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B115" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C115" s="20">
+        <v>16862</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B116" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C116" s="17">
+        <v>16798</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C117" s="20">
+        <v>91269</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C118" s="17">
+        <v>90721</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C119" s="20">
+        <v>89872</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C120" s="17">
+        <v>89556</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C121" s="20">
+        <v>89389</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B122" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C122" s="17">
+        <v>281206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B123" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C123" s="20">
+        <v>281753</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B124" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C124" s="17">
+        <v>286432</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B125" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C125" s="20">
+        <v>288589</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B126" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C126" s="17">
+        <v>290346</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B127" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C127" s="20">
+        <v>8684</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C128" s="17">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B129" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C129" s="20">
+        <v>8580</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B130" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C130" s="17">
+        <v>8540</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B131" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C131" s="20">
+        <v>8495</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B132" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C132" s="17">
+        <v>13312</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C133" s="20">
+        <v>13203</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B134" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C134" s="17">
+        <v>13092</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C135" s="20">
+        <v>13008</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B136" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C136" s="17">
+        <v>12882</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B137" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C137" s="20">
+        <v>440519</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B138" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C138" s="17">
+        <v>438729</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B139" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C139" s="20">
+        <v>437961</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B140" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C140" s="17">
+        <v>437174</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B141" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C141" s="20">
+        <v>436308</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B142" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C142" s="17">
+        <v>137999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C143" s="20">
+        <v>136923</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B144" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C144" s="17">
+        <v>135629</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B145" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C145" s="20">
+        <v>135107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B146" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C146" s="17">
+        <v>134913</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B147" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C147" s="20">
+        <v>102472</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C148" s="17">
+        <v>102405</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B149" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C149" s="20">
+        <v>101044</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B150" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C150" s="17">
+        <v>100711</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B151" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C151" s="20">
+        <v>100363</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B152" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C152" s="17">
+        <v>3187162</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B153" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C153" s="20">
+        <v>3163288</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B154" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C154" s="17">
+        <v>3159074</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B155" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C155" s="20">
+        <v>3148555</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B156" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C156" s="17">
+        <v>3150716</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B157" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C157" s="20">
+        <v>405794</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C158" s="17">
+        <v>408838</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B159" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C159" s="20">
+        <v>410770</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B160" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C160" s="17">
+        <v>413618</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B161" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C161" s="20">
+        <v>416014</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B162" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C162" s="17">
+        <v>19848</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B163" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C163" s="20">
+        <v>19719</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B164" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C164" s="17">
+        <v>19278</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B165" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C165" s="20">
+        <v>19078</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B166" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C166" s="17">
+        <v>18841</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B167" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C167" s="20">
+        <v>2422008</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B168" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C168" s="17">
+        <v>2430141</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B169" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C169" s="20">
+        <v>2439655</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B170" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C170" s="17">
+        <v>2451185</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B171" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C171" s="20">
+        <v>2455509</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B172" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C172" s="17">
+        <v>1586154</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B173" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C173" s="20">
+        <v>1582170</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B174" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C174" s="17">
+        <v>1575167</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B175" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C175" s="20">
+        <v>1578904</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B176" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C176" s="17">
+        <v>1583935</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B177" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C177" s="20">
+        <v>64337</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B178" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C178" s="17">
+        <v>65116</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B179" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C179" s="20">
+        <v>65883</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B180" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C180" s="17">
+        <v>65783</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B181" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C181" s="20">
+        <v>65798</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B182" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C182" s="17">
+        <v>2184801</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B183" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C183" s="20">
+        <v>2181371</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B184" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C184" s="17">
+        <v>2181980</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B185" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C185" s="20">
+        <v>2182369</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B186" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C186" s="17">
+        <v>2184474</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B187" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C187" s="20">
+        <v>3304281</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B188" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C188" s="17">
+        <v>3281991</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B189" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C189" s="20">
+        <v>3288754</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B190" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C190" s="17">
+        <v>3289885</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B191" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C191" s="20">
+        <v>3297545</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B192" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C192" s="17">
+        <v>871583</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B193" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C193" s="20">
+        <v>840454</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B194" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C194" s="17">
+        <v>839310</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B195" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C195" s="20">
+        <v>838251</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B196" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C196" s="17">
+        <v>837165</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B197" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C197" s="20">
+        <v>779717</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B198" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C198" s="17">
+        <v>782157</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B199" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C199" s="20">
+        <v>786585</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B200" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C200" s="17">
+        <v>792088</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B201" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C201" s="20">
+        <v>795790</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B202" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C202" s="17">
+        <v>282314</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B203" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C203" s="20">
+        <v>278343</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B204" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C204" s="17">
+        <v>280208</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B205" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C205" s="20">
+        <v>278976</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B206" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C206" s="17">
+        <v>278076</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B207" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C207" s="20">
+        <v>761474</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B208" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C208" s="17">
+        <v>748738</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B209" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C209" s="20">
+        <v>743000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B210" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C210" s="17">
+        <v>740929</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B211" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C211" s="20">
+        <v>740468</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B212" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C212" s="17">
+        <v>447566</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B213" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C213" s="20">
+        <v>438704</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B214" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C214" s="17">
+        <v>443893</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B215" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C215" s="20">
+        <v>442152</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B216" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C216" s="17">
+        <v>442648</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B217" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C217" s="20">
+        <v>1927909</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B218" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C218" s="17">
+        <v>1895854</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B219" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C219" s="20">
+        <v>1897174</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B220" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C220" s="17">
+        <v>1900834</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B221" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C221" s="20">
+        <v>1904477</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B222" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C222" s="17">
+        <v>271561</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B223" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C223" s="20">
+        <v>263413</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B224" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C224" s="17">
+        <v>265662</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B225" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C225" s="20">
+        <v>263775</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B226" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C226" s="17">
+        <v>262862</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B227" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C227" s="20">
+        <v>181956</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B228" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C228" s="17">
+        <v>181316</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B229" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C229" s="20">
+        <v>179759</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B230" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C230" s="17">
+        <v>179348</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B231" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C231" s="20">
+        <v>179723</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B232" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C232" s="17">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B233" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C233" s="20">
+        <v>3216</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B234" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C234" s="17">
+        <v>3195</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B235" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C235" s="20">
+        <v>3162</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B236" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C236" s="17">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B237" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C237" s="20">
+        <v>44002</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B238" s="16">
+        <v>2021</v>
+      </c>
+      <c r="C238" s="17">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B239" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C239" s="20">
+        <v>43397</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B240" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C240" s="17">
+        <v>43099</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B241" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C241" s="20">
+        <v>42882</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B242" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C242" s="17">
+        <v>452747</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B243" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C243" s="20">
+        <v>449411</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B244" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C244" s="17">
+        <v>446774</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B245" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C245" s="20">
+        <v>446763</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B246" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C246" s="17">
+        <v>447028</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B247" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C247" s="20">
+        <v>488361</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B248" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C248" s="17">
+        <v>483275</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B249" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C249" s="20">
+        <v>480783</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B250" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C250" s="17">
+        <v>479292</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B251" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C251" s="20">
+        <v>479237</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B252" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C252" s="17">
+        <v>553102</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B253" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C253" s="20">
+        <v>550689</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B254" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C254" s="17">
+        <v>548763</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B255" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C255" s="20">
+        <v>548838</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B256" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C256" s="17">
+        <v>550680</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B257" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C257" s="20">
+        <v>99481</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B258" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C258" s="17">
+        <v>99016</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B259" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C259" s="20">
+        <v>99399</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B260" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C260" s="17">
+        <v>99824</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B261" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C261" s="20">
+        <v>100071</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B262" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C262" s="17">
+        <v>65829</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B263" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C263" s="20">
+        <v>65465</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B264" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C264" s="17">
+        <v>65079</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B265" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C265" s="20">
+        <v>64786</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B266" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C266" s="17">
+        <v>64648</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B267" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C267" s="20">
+        <v>16103</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B268" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C268" s="17">
+        <v>16011</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B269" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C269" s="20">
+        <v>15928</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B270" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C270" s="17">
+        <v>15871</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B271" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C271" s="20">
+        <v>15807</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B272" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C272" s="17">
+        <v>472440</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B273" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C273" s="20">
+        <v>474525</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B274" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C274" s="17">
+        <v>476238</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B275" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C275" s="20">
+        <v>478192</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B276" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C276" s="17">
+        <v>480564</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B277" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C277" s="20">
+        <v>55445</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B278" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C278" s="17">
+        <v>54594</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B279" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C279" s="20">
+        <v>53141</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B280" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C280" s="17">
+        <v>53195</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B281" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C281" s="20">
+        <v>53004</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B282" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C282" s="17">
+        <v>844126</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B283" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C283" s="20">
+        <v>837763</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B284" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C284" s="17">
+        <v>831169</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B285" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C285" s="20">
+        <v>826745</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B286" s="16">
+        <v>2024</v>
+      </c>
+      <c r="C286" s="17">
+        <v>824051</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B287" s="19">
+        <v>2020</v>
+      </c>
+      <c r="C287" s="20">
+        <v>218271</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B288" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C288" s="17">
+        <v>214504</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B289" s="19">
+        <v>2022</v>
+      </c>
+      <c r="C289" s="20">
+        <v>221700</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B290" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C290" s="17">
+        <v>221202</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B291" s="19">
+        <v>2024</v>
+      </c>
+      <c r="C291" s="20">
+        <v>222326</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B292" s="16">
+        <v>2020</v>
+      </c>
+      <c r="C292" s="17">
+        <v>81831</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B293" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C293" s="20">
+        <v>82091</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B294" s="16">
+        <v>2022</v>
+      </c>
+      <c r="C294" s="17">
+        <v>82563</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B295" s="19">
+        <v>2023</v>
+      </c>
+      <c r="C295" s="20">
+        <v>83405</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A296" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B296" s="23">
+        <v>2024</v>
+      </c>
+      <c r="C296" s="24">
+        <v>83959</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DF17EE-2BF8-40BC-AD74-DCFC418889E9}">
   <dimension ref="A1:H237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="F191" sqref="F191"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E222" sqref="E222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3902,7 +7297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06019EA7-A7E8-440C-937E-715FF6003195}">
   <dimension ref="A1:H178"/>
   <sheetViews>

</xml_diff>